<commit_message>
add new word and modify AddShop&EditShop api
</commit_message>
<xml_diff>
--- a/Document/TABLE_DESIGN.xlsx
+++ b/Document/TABLE_DESIGN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xulez\source\repos\Order\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C37259A-139D-448A-9535-D1E0D6C52A95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1EFD2B-0608-4E43-B9D3-F50C2A91D439}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -325,6 +325,22 @@
   </si>
   <si>
     <t>CHAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IS_PRINT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否打印</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PERSON_NUM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1642,10 +1658,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C4DFAB-4DBA-4801-87C8-E514232C889F}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1808,6 +1824,28 @@
       </c>
       <c r="C10" s="10" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add log record & add new apis & fix bug
</commit_message>
<xml_diff>
--- a/Document/TABLE_DESIGN.xlsx
+++ b/Document/TABLE_DESIGN.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xulez\source\repos\Order\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1EFD2B-0608-4E43-B9D3-F50C2A91D439}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48A25E6-B108-4693-B815-3901FBA216EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="IMAGE" sheetId="9" r:id="rId1"/>
-    <sheet name="SHOP_DESK" sheetId="8" r:id="rId2"/>
-    <sheet name="SHOP" sheetId="7" r:id="rId3"/>
-    <sheet name="ORDER_DETAIL_FOOD" sheetId="6" r:id="rId4"/>
-    <sheet name="ORDER_DETAIL" sheetId="5" r:id="rId5"/>
-    <sheet name="ORDER_HEAD" sheetId="4" r:id="rId6"/>
-    <sheet name="FOOD_DETAIL" sheetId="3" r:id="rId7"/>
-    <sheet name="FOOD" sheetId="2" r:id="rId8"/>
-    <sheet name="FOOD_TYPE" sheetId="1" r:id="rId9"/>
+    <sheet name="LOGS" sheetId="10" r:id="rId1"/>
+    <sheet name="IMAGE" sheetId="9" r:id="rId2"/>
+    <sheet name="SHOP_DESK" sheetId="8" r:id="rId3"/>
+    <sheet name="SHOP" sheetId="7" r:id="rId4"/>
+    <sheet name="ORDER_DETAIL_FOOD" sheetId="6" r:id="rId5"/>
+    <sheet name="ORDER_DETAIL" sheetId="5" r:id="rId6"/>
+    <sheet name="ORDER_HEAD" sheetId="4" r:id="rId7"/>
+    <sheet name="FOOD_DETAIL" sheetId="3" r:id="rId8"/>
+    <sheet name="FOOD" sheetId="2" r:id="rId9"/>
+    <sheet name="FOOD_TYPE" sheetId="1" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -341,6 +342,26 @@
   </si>
   <si>
     <t>人数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PARAMS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请求参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(2000)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESPONSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回参数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -771,11 +792,353 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1300A995-5B53-48CA-97CE-EA6E2CE40961}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" customWidth="1"/>
+    <col min="5" max="5" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B25DCAC-0E1C-4043-9A26-06124A0732C7}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F7" sqref="A1:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -936,7 +1299,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B55D987-CB72-429E-AE72-2246DE839C12}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -1113,7 +1476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4A122D-5A1A-4419-B2B3-B15CC53D0104}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -1309,7 +1672,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E4C22E8-7A8A-4805-B530-F2ADE7E5B03B}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1494,7 +1857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A62B9A-1498-4753-AD48-BDF1D3B6CFE8}">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -1656,11 +2019,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C4DFAB-4DBA-4801-87C8-E514232C889F}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -1855,7 +2218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBD2768-37BB-49A9-BF80-4D37AD0F37EE}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -2043,7 +2406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5146F3A-85A4-4739-8CD1-C45EB909D3EB}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -2219,184 +2582,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" customWidth="1"/>
-    <col min="5" max="5" width="3.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="7"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>